<commit_message>
Some changes to lab notebook and ROIs: starting Neurosynth analysis
</commit_message>
<xml_diff>
--- a/Implicated_in_literature.xlsx
+++ b/Implicated_in_literature.xlsx
@@ -999,7 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -1708,8 +1708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H38"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2166,7 +2166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>